<commit_message>
BFS works from any starting pt
</commit_message>
<xml_diff>
--- a/Mapping_W1/Scale Layout.xlsx
+++ b/Mapping_W1/Scale Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fullstackmachine/Desktop/BevCode/AdvAlg_221/Mapping_W1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3005BE5-A26E-164B-AA4E-41EF092F1D4C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D064ABAD-F2B3-FF4F-99DA-356F39DBEA95}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10400" yWindow="2260" windowWidth="27640" windowHeight="15740" xr2:uid="{7847CF37-47B2-4644-97DD-7F9141894AA2}"/>
+    <workbookView xWindow="4960" yWindow="4440" windowWidth="27640" windowHeight="15740" xr2:uid="{7847CF37-47B2-4644-97DD-7F9141894AA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C27980-9AAC-4B4B-9E33-18D7A0AB4409}">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>